<commit_message>
SVN Revision #7055 by davidreddy       - Update Std design system maps and fan power per 3/3 CEC NACM system map document with corrections to fan power table.
</commit_message>
<xml_diff>
--- a/Documentation/T24N/FanPowerAllowances-T24N_2022.xlsx
+++ b/Documentation/T24N/FanPowerAllowances-T24N_2022.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CBECC\CBECC-Com_2022_OB360\Documentation\T24N\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CBECC\CBECC-Com_MFamRestructure\Documentation\T24N\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7F42EF-95E8-403C-A845-40FE616DF3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69A2E51-C107-4A88-BB00-EBC725C78833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="6330" windowWidth="29040" windowHeight="15840" xr2:uid="{6C0296AB-08E0-4615-A5BD-91F94E452329}"/>
+    <workbookView xWindow="7200" yWindow="1185" windowWidth="21600" windowHeight="11385" xr2:uid="{6C0296AB-08E0-4615-A5BD-91F94E452329}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t>Exhaust filters, scrubbers, or other exhaust treatment (calculation required, see note)</t>
   </si>
@@ -88,48 +88,12 @@
     <t>&gt;10000</t>
   </si>
   <si>
-    <t>1 – SZAC (with furnace)</t>
-  </si>
-  <si>
-    <t>3 – PSZ-HP (no furnace)</t>
-  </si>
-  <si>
-    <t>3 – PSZ-AC (with furnace)</t>
-  </si>
-  <si>
-    <t>5 – PVAV with reheat</t>
-  </si>
-  <si>
-    <t>6 – VAV with reheat</t>
-  </si>
-  <si>
-    <t>7 – SZ VAV (no furnace)</t>
-  </si>
-  <si>
-    <t>7 – SZ VAV (with furnace)</t>
-  </si>
-  <si>
-    <t>9 – Heating and Ventilation</t>
-  </si>
-  <si>
-    <t>Sys1</t>
-  </si>
-  <si>
-    <t>Sys4</t>
-  </si>
-  <si>
-    <t>Sys3</t>
-  </si>
-  <si>
     <t>Sys5</t>
   </si>
   <si>
     <t>Sys6</t>
   </si>
   <si>
-    <t>Sys7h</t>
-  </si>
-  <si>
     <t>Sys7a</t>
   </si>
   <si>
@@ -164,6 +128,48 @@
   </si>
   <si>
     <t>FullyDuctedRet</t>
+  </si>
+  <si>
+    <t>3a – SZAC</t>
+  </si>
+  <si>
+    <t>3b – SZHP (no furnace)</t>
+  </si>
+  <si>
+    <t>3c – SZDFHP (with furnace)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7a – SZVAVAC </t>
+  </si>
+  <si>
+    <t>7b – SZVAVHP</t>
+  </si>
+  <si>
+    <t>7c – SZVAVDFHP (with furnace)</t>
+  </si>
+  <si>
+    <t>5 – PVAV</t>
+  </si>
+  <si>
+    <t>6 – VAV</t>
+  </si>
+  <si>
+    <t>9 – HEATVENT</t>
+  </si>
+  <si>
+    <t>Sys3a</t>
+  </si>
+  <si>
+    <t>Sys3b</t>
+  </si>
+  <si>
+    <t>Sys3c</t>
+  </si>
+  <si>
+    <t>Sys7b</t>
+  </si>
+  <si>
+    <t>Sys7c</t>
   </si>
 </sst>
 </file>
@@ -525,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92DA6498-11F7-4E80-B1C0-60D82226771E}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,25 +544,25 @@
     <col min="4" max="11" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>0</v>
@@ -577,7 +583,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -585,16 +591,16 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
         <v>11</v>
@@ -609,12 +615,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>8.8999999999999996E-2</v>
@@ -641,12 +647,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D6" s="3">
         <v>0.1</v>
@@ -673,9 +679,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -705,12 +711,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D8" s="3">
         <v>9.0999999999999998E-2</v>
@@ -737,12 +743,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D9" s="3">
         <v>0.10199999999999999</v>
@@ -769,7 +775,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -801,85 +807,91 @@
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="G15" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H15" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="I15" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="J15" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="K15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="L15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D16">
-        <v>0.75600000000000001</v>
+        <v>0.80200000000000005</v>
       </c>
       <c r="E16">
         <v>0.74399999999999999</v>
@@ -888,27 +900,30 @@
         <v>0.80200000000000005</v>
       </c>
       <c r="G16">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="H16">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="I16">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="J16">
         <v>1</v>
       </c>
-      <c r="H16">
+      <c r="K16">
         <v>0.97699999999999998</v>
       </c>
-      <c r="I16">
-        <v>0.74399999999999999</v>
-      </c>
-      <c r="J16">
-        <v>0.80200000000000005</v>
-      </c>
-      <c r="K16">
+      <c r="L16">
         <v>0.61599999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D17">
-        <v>0.74</v>
+        <v>0.78</v>
       </c>
       <c r="E17">
         <v>0.72</v>
@@ -917,27 +932,30 @@
         <v>0.78</v>
       </c>
       <c r="G17">
+        <v>0.78</v>
+      </c>
+      <c r="H17">
+        <v>0.72</v>
+      </c>
+      <c r="I17">
+        <v>0.78</v>
+      </c>
+      <c r="J17">
         <v>1.022</v>
       </c>
-      <c r="H17">
+      <c r="K17">
         <v>1.0129999999999999</v>
       </c>
-      <c r="I17">
-        <v>0.72</v>
-      </c>
-      <c r="J17">
-        <v>0.78</v>
-      </c>
-      <c r="K17">
+      <c r="L17">
         <v>0.62</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>16</v>
       </c>
       <c r="D18">
-        <v>0.71199999999999997</v>
+        <v>0.748</v>
       </c>
       <c r="E18">
         <v>0.67600000000000005</v>
@@ -946,22 +964,25 @@
         <v>0.748</v>
       </c>
       <c r="G18">
+        <v>0.748</v>
+      </c>
+      <c r="H18">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="I18">
+        <v>0.748</v>
+      </c>
+      <c r="J18">
         <v>0.96399999999999997</v>
       </c>
-      <c r="H18">
+      <c r="K18">
         <v>0.94699999999999995</v>
       </c>
-      <c r="I18">
-        <v>0.67600000000000005</v>
-      </c>
-      <c r="J18">
-        <v>0.748</v>
-      </c>
-      <c r="K18">
+      <c r="L18">
         <v>0.60499999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
SVN Revision #7254 by davidreddy       Merged revision(s) from branches/CBECC_MFamRestructure_CentHVACForRC:
</commit_message>
<xml_diff>
--- a/Documentation/T24N/FanPowerAllowances-T24N_2022.xlsx
+++ b/Documentation/T24N/FanPowerAllowances-T24N_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CBECC\CBECC-Com_MFamRestructure\Documentation\T24N\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CBECC\CBECC-COM\CBECC-Com_2022_OB360\Documentation\T24N\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69A2E51-C107-4A88-BB00-EBC725C78833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41FB351-489F-45D1-8EA0-D1886497096D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1185" windowWidth="21600" windowHeight="11385" xr2:uid="{6C0296AB-08E0-4615-A5BD-91F94E452329}"/>
+    <workbookView xWindow="28680" yWindow="6330" windowWidth="29040" windowHeight="15840" xr2:uid="{6C0296AB-08E0-4615-A5BD-91F94E452329}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
   <si>
     <t>Exhaust filters, scrubbers, or other exhaust treatment (calculation required, see note)</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Biosafety cabinet (calculation required, see note)</t>
   </si>
   <si>
-    <t>Energy Recovery (Enthalpy Recovery Ratio ≥ 0.60 and &lt;0.65)  </t>
-  </si>
-  <si>
     <t>;</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
     <t>BiosftyCabExh</t>
   </si>
   <si>
-    <t>ERV</t>
-  </si>
-  <si>
     <t>Single Zone VAV Systems that are capable of turning down to 50% of full load airflow at a maximum of 30% design wattage</t>
   </si>
   <si>
@@ -170,6 +164,30 @@
   </si>
   <si>
     <t>Sys7c</t>
+  </si>
+  <si>
+    <t>Exhaust Systems Base Allowance</t>
+  </si>
+  <si>
+    <t>Supply - Energy Recovery (Enthalpy Recovery Ratio ? 0.60 and &lt;0.65)  </t>
+  </si>
+  <si>
+    <t>Return - Energy Recovery (Enthalpy Recovery Ratio ? 0.60 and &lt;0.65)  </t>
+  </si>
+  <si>
+    <t>Return - Filter (any MERV value)</t>
+  </si>
+  <si>
+    <t>ExhBaseAllow</t>
+  </si>
+  <si>
+    <t>ERVSupply</t>
+  </si>
+  <si>
+    <t>ERVReturn</t>
+  </si>
+  <si>
+    <t>RetFilter</t>
   </si>
 </sst>
 </file>
@@ -531,38 +549,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92DA6498-11F7-4E80-B1C0-60D82226771E}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20:I22"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="11" width="20" customWidth="1"/>
+    <col min="4" max="9" width="20" customWidth="1"/>
+    <col min="10" max="14" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>0</v>
@@ -577,50 +596,68 @@
         <v>3</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>11</v>
       </c>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="J4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N4" t="s">
         <v>13</v>
       </c>
-      <c r="K4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5" s="3">
         <v>8.8999999999999996E-2</v>
@@ -640,19 +677,28 @@
       <c r="I5" s="3">
         <v>0.17699999999999999</v>
       </c>
-      <c r="J5" s="3">
-        <v>0.374</v>
-      </c>
-      <c r="K5" s="3">
+      <c r="J5">
+        <v>0.221</v>
+      </c>
+      <c r="K5">
+        <v>0.184</v>
+      </c>
+      <c r="L5">
+        <v>0.19</v>
+      </c>
+      <c r="M5">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="N5" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3">
         <v>0.1</v>
@@ -672,19 +718,28 @@
       <c r="I6" s="3">
         <v>0.19800000000000001</v>
       </c>
-      <c r="J6" s="3">
-        <v>0.318</v>
-      </c>
-      <c r="K6" s="3">
+      <c r="J6">
+        <v>0.246</v>
+      </c>
+      <c r="K6">
+        <v>0.155</v>
+      </c>
+      <c r="L6">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="M6">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="N6" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3">
         <v>0.11600000000000001</v>
@@ -704,19 +759,28 @@
       <c r="I7" s="3">
         <v>0.23100000000000001</v>
       </c>
-      <c r="J7" s="3">
-        <v>0.28899999999999998</v>
-      </c>
-      <c r="K7" s="3">
+      <c r="J7">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="K7">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="L7">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="M7">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="N7" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D8" s="3">
         <v>9.0999999999999998E-2</v>
@@ -736,19 +800,28 @@
       <c r="I8" s="3">
         <v>0.17899999999999999</v>
       </c>
-      <c r="J8" s="3">
-        <v>0.38100000000000001</v>
-      </c>
-      <c r="K8" s="3">
+      <c r="J8">
+        <v>0.186</v>
+      </c>
+      <c r="K8">
+        <v>0.19</v>
+      </c>
+      <c r="L8">
+        <v>0.191</v>
+      </c>
+      <c r="M8">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="N8" s="3">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D9" s="3">
         <v>0.10199999999999999</v>
@@ -768,19 +841,28 @@
       <c r="I9" s="3">
         <v>0.20200000000000001</v>
       </c>
-      <c r="J9" s="3">
-        <v>0.32900000000000001</v>
-      </c>
-      <c r="K9" s="3">
+      <c r="J9">
+        <v>0.184</v>
+      </c>
+      <c r="K9">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="L9">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="M9">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="N9" s="3">
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10" s="3">
         <v>0.11600000000000001</v>
@@ -800,95 +882,104 @@
       <c r="I10" s="3">
         <v>0.23200000000000001</v>
       </c>
-      <c r="J10" s="3">
-        <v>0.29299999999999998</v>
-      </c>
-      <c r="K10" s="3">
+      <c r="J10">
+        <v>0.19</v>
+      </c>
+      <c r="K10">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="L10">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="M10">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="N10" s="3">
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" t="s">
+        <v>36</v>
+      </c>
+      <c r="L14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" t="s">
-        <v>36</v>
-      </c>
-      <c r="J14" t="s">
-        <v>37</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="D15" t="s">
         <v>38</v>
       </c>
-      <c r="L14" t="s">
+      <c r="E15" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="F15" t="s">
         <v>40</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" t="s">
         <v>41</v>
       </c>
-      <c r="F15" t="s">
+      <c r="I15" t="s">
         <v>42</v>
       </c>
-      <c r="G15" t="s">
+      <c r="J15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" t="s">
+        <v>16</v>
+      </c>
+      <c r="L15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
         <v>19</v>
-      </c>
-      <c r="H15" t="s">
-        <v>43</v>
-      </c>
-      <c r="I15" t="s">
-        <v>44</v>
-      </c>
-      <c r="J15" t="s">
-        <v>17</v>
-      </c>
-      <c r="K15" t="s">
-        <v>18</v>
-      </c>
-      <c r="L15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>21</v>
       </c>
       <c r="D16">
         <v>0.80200000000000005</v>
@@ -920,7 +1011,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D17">
         <v>0.78</v>
@@ -952,7 +1043,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D18">
         <v>0.748</v>
@@ -984,7 +1075,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>